<commit_message>
fiz o calcula desconto
</commit_message>
<xml_diff>
--- a/Modelos UML/Descrição UseCases/EscolherPacote.xlsx
+++ b/Modelos UML/Descrição UseCases/EscolherPacote.xlsx
@@ -84,9 +84,6 @@
     <t>8. Regista e verifica componentes adicionais</t>
   </si>
   <si>
-    <t>9. Calcula desconto</t>
-  </si>
-  <si>
     <t>Alternativa 1 [Componentes inválidos] (passo 7)</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>11.1 Não confirma</t>
+  </si>
+  <si>
+    <t>9. Calcula preço</t>
   </si>
 </sst>
 </file>
@@ -707,7 +707,7 @@
   <dimension ref="B1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -826,20 +826,20 @@
       <c r="B15" s="20"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="20"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="20"/>
       <c r="C17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -847,37 +847,37 @@
       <c r="B18" s="20"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="20"/>
       <c r="C19" s="5"/>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="14"/>
       <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="14"/>
       <c r="C22" s="5"/>
       <c r="D22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -887,10 +887,10 @@
     </row>
     <row r="24" spans="2:4" s="11" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="D24" s="10"/>
     </row>
@@ -898,7 +898,7 @@
       <c r="B25" s="14"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="2:4" s="11" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Criei o DAO para peca e carro. Carro ainda esta incompleto
</commit_message>
<xml_diff>
--- a/Modelos UML/Descrição UseCases/EscolherPacote.xlsx
+++ b/Modelos UML/Descrição UseCases/EscolherPacote.xlsx
@@ -105,9 +105,6 @@
     <t>12. Regista confirmação</t>
   </si>
   <si>
-    <t xml:space="preserve">13. Insere carro na fila de produção </t>
-  </si>
-  <si>
     <t>Alternativa 2 [Não confirma] (passo 11)</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>9. Calcula preço</t>
+  </si>
+  <si>
+    <t>13. Insere carro no sistema</t>
   </si>
 </sst>
 </file>
@@ -707,7 +707,7 @@
   <dimension ref="B1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -826,7 +826,7 @@
       <c r="B15" s="20"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -854,7 +854,7 @@
       <c r="B19" s="20"/>
       <c r="C19" s="5"/>
       <c r="D19" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -887,10 +887,10 @@
     </row>
     <row r="24" spans="2:4" s="11" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>28</v>
       </c>
       <c r="D24" s="10"/>
     </row>

</xml_diff>

<commit_message>
Corrigi alguns detalhes nos diagramas
</commit_message>
<xml_diff>
--- a/Modelos UML/Descrição UseCases/EscolherPacote.xlsx
+++ b/Modelos UML/Descrição UseCases/EscolherPacote.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\Luís\3º ano\1º Semestre\DSS\Trabalho\DSS\Modelos UML\Descrição UseCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmcca\Documents\3º Ano\DSS\Trabalho\DSS\DSS\Modelos UML\Descrição UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E71627-9499-4C01-9CCB-88F7F77E572B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,9 +79,6 @@
     <t>6. Mostra componentes usados</t>
   </si>
   <si>
-    <t>7. Escolhe especificações adicionais e (ou não) altera pacote</t>
-  </si>
-  <si>
     <t>8. Regista e verifica componentes adicionais</t>
   </si>
   <si>
@@ -115,12 +113,15 @@
   </si>
   <si>
     <t>13. Insere carro no sistema</t>
+  </si>
+  <si>
+    <t>7. Escolhe especificações adicionais</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -703,11 +704,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -811,7 +812,7 @@
     <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="20"/>
       <c r="C13" s="5" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -819,27 +820,27 @@
       <c r="B14" s="20"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="20"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="20"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="20"/>
       <c r="C17" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -847,37 +848,37 @@
       <c r="B18" s="20"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="20"/>
       <c r="C19" s="5"/>
       <c r="D19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="14"/>
       <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="14"/>
       <c r="C22" s="5"/>
       <c r="D22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -887,10 +888,10 @@
     </row>
     <row r="24" spans="2:4" s="11" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>27</v>
       </c>
       <c r="D24" s="10"/>
     </row>
@@ -898,7 +899,7 @@
       <c r="B25" s="14"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="2:4" s="11" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>